<commit_message>
small adhoc fix to pandas issue in databaseAux.py
</commit_message>
<xml_diff>
--- a/Data/0_GlobalData.xlsx
+++ b/Data/0_GlobalData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="2" r:id="rId1"/>
@@ -605,7 +605,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,7 +725,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,8 +1202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,7 +1293,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,7 +1332,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,8 +1813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>